<commit_message>
added to validation rules document
</commit_message>
<xml_diff>
--- a/PIT3/validation-rules/Employer_Submission_RPN_Validation_Rules.xlsx
+++ b/PIT3/validation-rules/Employer_Submission_RPN_Validation_Rules.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2931796C-8020-49F7-9E82-F67D7F6368AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294E2B46-C888-47A2-B9A7-0B7C96ADE6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Control" sheetId="5" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ValidationRules!$G$1:$G$480</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Document Control'!$A$1:$E$32</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">ValidationRules!$A$1:$M$148</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">ValidationRules!$A$1:$M$149</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">ValidationRules!$1:$1</definedName>
     <definedName name="ValidationCodes">#REF!</definedName>
   </definedNames>
@@ -22266,7 +22266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B8:M72"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -22990,7 +22990,7 @@
   </sheetPr>
   <dimension ref="A1:BN480"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -24355,8 +24355,8 @@
       <c r="M25" s="31" t="s">
         <v>298</v>
       </c>
-      <c r="N25" s="32" t="s">
-        <v>61</v>
+      <c r="N25" s="64" t="s">
+        <v>12</v>
       </c>
       <c r="O25" s="64" t="s">
         <v>12</v>
@@ -28674,8 +28674,8 @@
       <c r="M84" s="31" t="s">
         <v>298</v>
       </c>
-      <c r="N84" s="32" t="s">
-        <v>61</v>
+      <c r="N84" s="64" t="s">
+        <v>12</v>
       </c>
       <c r="O84" s="64" t="s">
         <v>12</v>
@@ -30031,8 +30031,8 @@
       <c r="M100" s="31" t="s">
         <v>298</v>
       </c>
-      <c r="N100" s="30" t="s">
-        <v>60</v>
+      <c r="N100" s="64" t="s">
+        <v>12</v>
       </c>
       <c r="O100" s="64" t="s">
         <v>12</v>
@@ -32132,318 +32132,318 @@
       <c r="BM123" s="21"/>
       <c r="BN123" s="21"/>
     </row>
-    <row r="124" spans="1:66" s="50" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A124" s="107" t="s">
+    <row r="124" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="8">
+        <v>168</v>
+      </c>
+      <c r="B124" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C124" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="D124" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E124" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F124" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G124" s="8">
+        <v>401</v>
+      </c>
+      <c r="H124" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="I124" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="J124" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="K124" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="L124" s="8">
+        <v>1014</v>
+      </c>
+      <c r="M124" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="N124" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="O124" s="64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="125" spans="1:66" s="50" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A125" s="107" t="s">
         <v>145</v>
       </c>
-      <c r="B124" s="107"/>
-      <c r="C124" s="107"/>
-      <c r="D124" s="107"/>
-      <c r="E124" s="107"/>
-      <c r="F124" s="107"/>
-      <c r="G124" s="107"/>
-      <c r="H124" s="107"/>
-      <c r="I124" s="107"/>
-      <c r="J124" s="107"/>
-      <c r="K124" s="107"/>
-      <c r="L124" s="107"/>
-      <c r="M124" s="107"/>
-      <c r="N124" s="107"/>
-      <c r="O124" s="107"/>
-      <c r="P124" s="21"/>
-      <c r="Q124" s="21"/>
-      <c r="R124" s="21"/>
-      <c r="S124" s="21"/>
-      <c r="T124" s="21"/>
-      <c r="U124" s="21"/>
-      <c r="V124" s="21"/>
-      <c r="W124" s="21"/>
-      <c r="X124" s="21"/>
-      <c r="Y124" s="21"/>
-      <c r="Z124" s="21"/>
-      <c r="AA124" s="21"/>
-      <c r="AB124" s="21"/>
-      <c r="AC124" s="21"/>
-      <c r="AD124" s="21"/>
-      <c r="AE124" s="21"/>
-      <c r="AF124" s="21"/>
-      <c r="AG124" s="21"/>
-      <c r="AH124" s="21"/>
-      <c r="AI124" s="21"/>
-      <c r="AJ124" s="21"/>
-      <c r="AK124" s="21"/>
-      <c r="AL124" s="21"/>
-      <c r="AM124" s="21"/>
-      <c r="AN124" s="21"/>
-      <c r="AO124" s="21"/>
-      <c r="AP124" s="21"/>
-      <c r="AQ124" s="21"/>
-      <c r="AR124" s="21"/>
-      <c r="AS124" s="21"/>
-      <c r="AT124" s="21"/>
-      <c r="AU124" s="21"/>
-      <c r="AV124" s="21"/>
-      <c r="AW124" s="21"/>
-      <c r="AX124" s="21"/>
-      <c r="AY124" s="21"/>
-      <c r="AZ124" s="21"/>
-      <c r="BA124" s="21"/>
-      <c r="BB124" s="21"/>
-      <c r="BC124" s="21"/>
-      <c r="BD124" s="21"/>
-      <c r="BE124" s="21"/>
-      <c r="BF124" s="21"/>
-      <c r="BG124" s="21"/>
-      <c r="BH124" s="21"/>
-      <c r="BI124" s="21"/>
-      <c r="BJ124" s="21"/>
-      <c r="BK124" s="21"/>
-      <c r="BL124" s="21"/>
-      <c r="BM124" s="21"/>
-      <c r="BN124" s="21"/>
-    </row>
-    <row r="125" spans="1:66" s="36" customFormat="1" ht="49.7" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A125" s="38">
+      <c r="B125" s="107"/>
+      <c r="C125" s="107"/>
+      <c r="D125" s="107"/>
+      <c r="E125" s="107"/>
+      <c r="F125" s="107"/>
+      <c r="G125" s="107"/>
+      <c r="H125" s="107"/>
+      <c r="I125" s="107"/>
+      <c r="J125" s="107"/>
+      <c r="K125" s="107"/>
+      <c r="L125" s="107"/>
+      <c r="M125" s="107"/>
+      <c r="N125" s="107"/>
+      <c r="O125" s="107"/>
+      <c r="P125" s="21"/>
+      <c r="Q125" s="21"/>
+      <c r="R125" s="21"/>
+      <c r="S125" s="21"/>
+      <c r="T125" s="21"/>
+      <c r="U125" s="21"/>
+      <c r="V125" s="21"/>
+      <c r="W125" s="21"/>
+      <c r="X125" s="21"/>
+      <c r="Y125" s="21"/>
+      <c r="Z125" s="21"/>
+      <c r="AA125" s="21"/>
+      <c r="AB125" s="21"/>
+      <c r="AC125" s="21"/>
+      <c r="AD125" s="21"/>
+      <c r="AE125" s="21"/>
+      <c r="AF125" s="21"/>
+      <c r="AG125" s="21"/>
+      <c r="AH125" s="21"/>
+      <c r="AI125" s="21"/>
+      <c r="AJ125" s="21"/>
+      <c r="AK125" s="21"/>
+      <c r="AL125" s="21"/>
+      <c r="AM125" s="21"/>
+      <c r="AN125" s="21"/>
+      <c r="AO125" s="21"/>
+      <c r="AP125" s="21"/>
+      <c r="AQ125" s="21"/>
+      <c r="AR125" s="21"/>
+      <c r="AS125" s="21"/>
+      <c r="AT125" s="21"/>
+      <c r="AU125" s="21"/>
+      <c r="AV125" s="21"/>
+      <c r="AW125" s="21"/>
+      <c r="AX125" s="21"/>
+      <c r="AY125" s="21"/>
+      <c r="AZ125" s="21"/>
+      <c r="BA125" s="21"/>
+      <c r="BB125" s="21"/>
+      <c r="BC125" s="21"/>
+      <c r="BD125" s="21"/>
+      <c r="BE125" s="21"/>
+      <c r="BF125" s="21"/>
+      <c r="BG125" s="21"/>
+      <c r="BH125" s="21"/>
+      <c r="BI125" s="21"/>
+      <c r="BJ125" s="21"/>
+      <c r="BK125" s="21"/>
+      <c r="BL125" s="21"/>
+      <c r="BM125" s="21"/>
+      <c r="BN125" s="21"/>
+    </row>
+    <row r="126" spans="1:66" s="36" customFormat="1" ht="49.7" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A126" s="38">
         <v>145</v>
-      </c>
-      <c r="B125" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="C125" s="41" t="s">
-        <v>241</v>
-      </c>
-      <c r="D125" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E125" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="F125" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="G125" s="24">
-        <v>400</v>
-      </c>
-      <c r="H125" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="I125" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="J125" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="K125" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="L125" s="86">
-        <v>3008</v>
-      </c>
-      <c r="M125" s="37" t="s">
-        <v>241</v>
-      </c>
-      <c r="N125" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="O125" s="87" t="s">
-        <v>242</v>
-      </c>
-      <c r="P125" s="35"/>
-      <c r="Q125" s="35"/>
-      <c r="R125" s="35"/>
-      <c r="S125" s="35"/>
-      <c r="T125" s="35"/>
-      <c r="U125" s="35"/>
-      <c r="V125" s="35"/>
-      <c r="W125" s="35"/>
-      <c r="X125" s="35"/>
-      <c r="Y125" s="35"/>
-      <c r="Z125" s="35"/>
-      <c r="AA125" s="35"/>
-      <c r="AB125" s="35"/>
-      <c r="AC125" s="35"/>
-      <c r="AD125" s="35"/>
-      <c r="AE125" s="35"/>
-      <c r="AF125" s="35"/>
-      <c r="AG125" s="35"/>
-      <c r="AH125" s="35"/>
-      <c r="AI125" s="35"/>
-      <c r="AJ125" s="35"/>
-      <c r="AK125" s="35"/>
-      <c r="AL125" s="35"/>
-      <c r="AM125" s="35"/>
-      <c r="AN125" s="35"/>
-      <c r="AO125" s="35"/>
-      <c r="AP125" s="35"/>
-      <c r="AQ125" s="35"/>
-      <c r="AR125" s="35"/>
-      <c r="AS125" s="35"/>
-      <c r="AT125" s="35"/>
-      <c r="AU125" s="35"/>
-      <c r="AV125" s="35"/>
-      <c r="AW125" s="35"/>
-      <c r="AX125" s="35"/>
-      <c r="AY125" s="35"/>
-      <c r="AZ125" s="35"/>
-      <c r="BA125" s="35"/>
-      <c r="BB125" s="35"/>
-      <c r="BC125" s="35"/>
-      <c r="BD125" s="35"/>
-      <c r="BE125" s="35"/>
-      <c r="BF125" s="35"/>
-      <c r="BG125" s="35"/>
-      <c r="BH125" s="35"/>
-      <c r="BI125" s="35"/>
-      <c r="BJ125" s="35"/>
-      <c r="BK125" s="35"/>
-      <c r="BL125" s="35"/>
-      <c r="BM125" s="35"/>
-      <c r="BN125" s="35"/>
-    </row>
-    <row r="126" spans="1:66" s="7" customFormat="1" ht="31.5" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A126" s="4">
-        <v>85</v>
       </c>
       <c r="B126" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="C126" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D126" s="4">
-        <v>8</v>
+      <c r="C126" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="D126" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="E126" s="24" t="s">
         <v>140</v>
       </c>
       <c r="F126" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="G126" s="44">
-        <v>200</v>
+        <v>141</v>
+      </c>
+      <c r="G126" s="24">
+        <v>400</v>
       </c>
       <c r="H126" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I126" s="24" t="s">
-        <v>227</v>
-      </c>
-      <c r="J126" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="J126" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="K126" s="4" t="s">
+      <c r="K126" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="L126" s="4">
-        <v>1010</v>
-      </c>
-      <c r="M126" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="N126" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="O126" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="P126" s="22"/>
-      <c r="Q126" s="22"/>
-      <c r="R126" s="22"/>
-      <c r="S126" s="22"/>
-      <c r="T126" s="22"/>
-      <c r="U126" s="22"/>
-      <c r="V126" s="22"/>
-      <c r="W126" s="22"/>
-      <c r="X126" s="22"/>
-      <c r="Y126" s="22"/>
-      <c r="Z126" s="22"/>
-      <c r="AA126" s="22"/>
-      <c r="AB126" s="22"/>
-      <c r="AC126" s="22"/>
-      <c r="AD126" s="22"/>
-      <c r="AE126" s="22"/>
-      <c r="AF126" s="22"/>
-      <c r="AG126" s="22"/>
-      <c r="AH126" s="22"/>
-      <c r="AI126" s="22"/>
-      <c r="AJ126" s="22"/>
-      <c r="AK126" s="22"/>
-      <c r="AL126" s="22"/>
-      <c r="AM126" s="22"/>
-      <c r="AN126" s="22"/>
-      <c r="AO126" s="22"/>
-      <c r="AP126" s="22"/>
-      <c r="AQ126" s="22"/>
-      <c r="AR126" s="22"/>
-      <c r="AS126" s="22"/>
-      <c r="AT126" s="22"/>
-      <c r="AU126" s="22"/>
-      <c r="AV126" s="22"/>
-      <c r="AW126" s="22"/>
-      <c r="AX126" s="22"/>
-      <c r="AY126" s="22"/>
-      <c r="AZ126" s="22"/>
-      <c r="BA126" s="22"/>
-      <c r="BB126" s="22"/>
-      <c r="BC126" s="22"/>
-      <c r="BD126" s="22"/>
-      <c r="BE126" s="22"/>
-      <c r="BF126" s="22"/>
-      <c r="BG126" s="22"/>
-      <c r="BH126" s="22"/>
-      <c r="BI126" s="22"/>
-      <c r="BJ126" s="22"/>
-      <c r="BK126" s="22"/>
-      <c r="BL126" s="22"/>
-      <c r="BM126" s="22"/>
-      <c r="BN126" s="22"/>
-    </row>
-    <row r="127" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="8">
-        <v>168</v>
+      <c r="L126" s="86">
+        <v>3008</v>
+      </c>
+      <c r="M126" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="N126" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="O126" s="87" t="s">
+        <v>242</v>
+      </c>
+      <c r="P126" s="35"/>
+      <c r="Q126" s="35"/>
+      <c r="R126" s="35"/>
+      <c r="S126" s="35"/>
+      <c r="T126" s="35"/>
+      <c r="U126" s="35"/>
+      <c r="V126" s="35"/>
+      <c r="W126" s="35"/>
+      <c r="X126" s="35"/>
+      <c r="Y126" s="35"/>
+      <c r="Z126" s="35"/>
+      <c r="AA126" s="35"/>
+      <c r="AB126" s="35"/>
+      <c r="AC126" s="35"/>
+      <c r="AD126" s="35"/>
+      <c r="AE126" s="35"/>
+      <c r="AF126" s="35"/>
+      <c r="AG126" s="35"/>
+      <c r="AH126" s="35"/>
+      <c r="AI126" s="35"/>
+      <c r="AJ126" s="35"/>
+      <c r="AK126" s="35"/>
+      <c r="AL126" s="35"/>
+      <c r="AM126" s="35"/>
+      <c r="AN126" s="35"/>
+      <c r="AO126" s="35"/>
+      <c r="AP126" s="35"/>
+      <c r="AQ126" s="35"/>
+      <c r="AR126" s="35"/>
+      <c r="AS126" s="35"/>
+      <c r="AT126" s="35"/>
+      <c r="AU126" s="35"/>
+      <c r="AV126" s="35"/>
+      <c r="AW126" s="35"/>
+      <c r="AX126" s="35"/>
+      <c r="AY126" s="35"/>
+      <c r="AZ126" s="35"/>
+      <c r="BA126" s="35"/>
+      <c r="BB126" s="35"/>
+      <c r="BC126" s="35"/>
+      <c r="BD126" s="35"/>
+      <c r="BE126" s="35"/>
+      <c r="BF126" s="35"/>
+      <c r="BG126" s="35"/>
+      <c r="BH126" s="35"/>
+      <c r="BI126" s="35"/>
+      <c r="BJ126" s="35"/>
+      <c r="BK126" s="35"/>
+      <c r="BL126" s="35"/>
+      <c r="BM126" s="35"/>
+      <c r="BN126" s="35"/>
+    </row>
+    <row r="127" spans="1:66" s="7" customFormat="1" ht="31.5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A127" s="4">
+        <v>85</v>
       </c>
       <c r="B127" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="C127" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="D127" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E127" s="8" t="s">
+      <c r="C127" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D127" s="4">
+        <v>8</v>
+      </c>
+      <c r="E127" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="F127" s="8" t="s">
+      <c r="F127" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="G127" s="8">
-        <v>401</v>
-      </c>
-      <c r="H127" s="54" t="s">
-        <v>216</v>
+      <c r="G127" s="44">
+        <v>200</v>
+      </c>
+      <c r="H127" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="I127" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="J127" s="92" t="s">
+        <v>227</v>
+      </c>
+      <c r="J127" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K127" s="92" t="s">
-        <v>32</v>
-      </c>
-      <c r="L127" s="8">
-        <v>1014</v>
-      </c>
-      <c r="M127" s="31" t="s">
-        <v>298</v>
+      <c r="K127" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L127" s="4">
+        <v>1010</v>
+      </c>
+      <c r="M127" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="N127" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="O127" s="64" t="s">
-        <v>12</v>
-      </c>
+      <c r="O127" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="P127" s="22"/>
+      <c r="Q127" s="22"/>
+      <c r="R127" s="22"/>
+      <c r="S127" s="22"/>
+      <c r="T127" s="22"/>
+      <c r="U127" s="22"/>
+      <c r="V127" s="22"/>
+      <c r="W127" s="22"/>
+      <c r="X127" s="22"/>
+      <c r="Y127" s="22"/>
+      <c r="Z127" s="22"/>
+      <c r="AA127" s="22"/>
+      <c r="AB127" s="22"/>
+      <c r="AC127" s="22"/>
+      <c r="AD127" s="22"/>
+      <c r="AE127" s="22"/>
+      <c r="AF127" s="22"/>
+      <c r="AG127" s="22"/>
+      <c r="AH127" s="22"/>
+      <c r="AI127" s="22"/>
+      <c r="AJ127" s="22"/>
+      <c r="AK127" s="22"/>
+      <c r="AL127" s="22"/>
+      <c r="AM127" s="22"/>
+      <c r="AN127" s="22"/>
+      <c r="AO127" s="22"/>
+      <c r="AP127" s="22"/>
+      <c r="AQ127" s="22"/>
+      <c r="AR127" s="22"/>
+      <c r="AS127" s="22"/>
+      <c r="AT127" s="22"/>
+      <c r="AU127" s="22"/>
+      <c r="AV127" s="22"/>
+      <c r="AW127" s="22"/>
+      <c r="AX127" s="22"/>
+      <c r="AY127" s="22"/>
+      <c r="AZ127" s="22"/>
+      <c r="BA127" s="22"/>
+      <c r="BB127" s="22"/>
+      <c r="BC127" s="22"/>
+      <c r="BD127" s="22"/>
+      <c r="BE127" s="22"/>
+      <c r="BF127" s="22"/>
+      <c r="BG127" s="22"/>
+      <c r="BH127" s="22"/>
+      <c r="BI127" s="22"/>
+      <c r="BJ127" s="22"/>
+      <c r="BK127" s="22"/>
+      <c r="BL127" s="22"/>
+      <c r="BM127" s="22"/>
+      <c r="BN127" s="22"/>
     </row>
     <row r="128" spans="1:66" s="7" customFormat="1" ht="18.75" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A128" s="106" t="s">
@@ -33731,92 +33731,92 @@
       <c r="N144" s="33"/>
       <c r="O144" s="33"/>
     </row>
-    <row r="145" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A145" s="107" t="s">
+    <row r="145" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A145" s="8">
+        <v>169</v>
+      </c>
+      <c r="B145" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="C145" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="D145" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E145" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F145" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G145" s="8">
+        <v>401</v>
+      </c>
+      <c r="H145" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="I145" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="J145" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="K145" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="L145" s="8">
+        <v>1014</v>
+      </c>
+      <c r="M145" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="N145" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="O145" s="64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="146" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A146" s="107" t="s">
         <v>145</v>
       </c>
-      <c r="B145" s="107"/>
-      <c r="C145" s="107"/>
-      <c r="D145" s="107"/>
-      <c r="E145" s="107"/>
-      <c r="F145" s="107"/>
-      <c r="G145" s="107"/>
-      <c r="H145" s="107"/>
-      <c r="I145" s="107"/>
-      <c r="J145" s="107"/>
-      <c r="K145" s="107"/>
-      <c r="L145" s="107"/>
-      <c r="M145" s="107"/>
-      <c r="N145" s="107"/>
-      <c r="O145" s="107"/>
-    </row>
-    <row r="146" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A146" s="4">
+      <c r="B146" s="107"/>
+      <c r="C146" s="107"/>
+      <c r="D146" s="107"/>
+      <c r="E146" s="107"/>
+      <c r="F146" s="107"/>
+      <c r="G146" s="107"/>
+      <c r="H146" s="107"/>
+      <c r="I146" s="107"/>
+      <c r="J146" s="107"/>
+      <c r="K146" s="107"/>
+      <c r="L146" s="107"/>
+      <c r="M146" s="107"/>
+      <c r="N146" s="107"/>
+      <c r="O146" s="107"/>
+    </row>
+    <row r="147" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A147" s="4">
         <v>154</v>
-      </c>
-      <c r="B146" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="C146" s="49" t="s">
-        <v>274</v>
-      </c>
-      <c r="D146" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E146" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F146" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G146" s="4">
-        <v>200</v>
-      </c>
-      <c r="H146" s="24" t="s">
-        <v>217</v>
-      </c>
-      <c r="I146" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="J146" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K146" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L146" s="4">
-        <v>4006</v>
-      </c>
-      <c r="M146" s="49" t="s">
-        <v>274</v>
-      </c>
-      <c r="N146" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="O146" s="49" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="147" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A147" s="8">
-        <v>151</v>
       </c>
       <c r="B147" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="C147" s="96" t="s">
-        <v>268</v>
+      <c r="C147" s="49" t="s">
+        <v>274</v>
       </c>
       <c r="D147" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E147" s="5" t="s">
+      <c r="E147" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F147" s="5" t="s">
+      <c r="F147" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="G147" s="38">
+      <c r="G147" s="4">
         <v>200</v>
       </c>
       <c r="H147" s="24" t="s">
@@ -33831,28 +33831,28 @@
       <c r="K147" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L147" s="8">
-        <v>4005</v>
-      </c>
-      <c r="M147" s="96" t="s">
-        <v>268</v>
+      <c r="L147" s="4">
+        <v>4006</v>
+      </c>
+      <c r="M147" s="49" t="s">
+        <v>274</v>
       </c>
       <c r="N147" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="O147" s="96" t="s">
-        <v>267</v>
+      <c r="O147" s="49" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="148" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A148" s="4">
-        <v>97</v>
+      <c r="A148" s="8">
+        <v>151</v>
       </c>
       <c r="B148" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="C148" s="23" t="s">
-        <v>85</v>
+      <c r="C148" s="96" t="s">
+        <v>268</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>12</v>
@@ -33875,33 +33875,33 @@
       <c r="J148" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K148" s="5" t="s">
-        <v>30</v>
+      <c r="K148" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="L148" s="8">
-        <v>4002</v>
-      </c>
-      <c r="M148" s="32" t="s">
-        <v>38</v>
+        <v>4005</v>
+      </c>
+      <c r="M148" s="96" t="s">
+        <v>268</v>
       </c>
       <c r="N148" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="O148" s="31" t="s">
-        <v>62</v>
+      <c r="O148" s="96" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="149" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B149" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="C149" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="D149" s="26" t="s">
+      <c r="C149" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D149" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E149" s="5" t="s">
@@ -33922,31 +33922,31 @@
       <c r="J149" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K149" s="26" t="s">
+      <c r="K149" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L149" s="26">
-        <v>4003</v>
+      <c r="L149" s="8">
+        <v>4002</v>
       </c>
       <c r="M149" s="32" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="N149" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="O149" s="33" t="s">
-        <v>1</v>
+      <c r="O149" s="31" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="150" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B150" s="31" t="s">
         <v>133</v>
       </c>
       <c r="C150" s="27" t="s">
-        <v>183</v>
+        <v>81</v>
       </c>
       <c r="D150" s="26" t="s">
         <v>12</v>
@@ -33973,35 +33973,35 @@
         <v>30</v>
       </c>
       <c r="L150" s="26">
-        <v>4004</v>
+        <v>4003</v>
       </c>
       <c r="M150" s="32" t="s">
-        <v>183</v>
+        <v>82</v>
       </c>
       <c r="N150" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="O150" s="31" t="s">
-        <v>184</v>
+      <c r="O150" s="33" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B151" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="C151" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D151" s="4">
-        <v>8</v>
-      </c>
-      <c r="E151" s="24" t="s">
+      <c r="C151" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="D151" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E151" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="F151" s="24" t="s">
+      <c r="F151" s="5" t="s">
         <v>140</v>
       </c>
       <c r="G151" s="38">
@@ -34013,70 +34013,70 @@
       <c r="I151" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="J151" s="4" t="s">
+      <c r="J151" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K151" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L151" s="4">
-        <v>1010</v>
-      </c>
-      <c r="M151" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="N151" s="30" t="s">
+      <c r="K151" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="L151" s="26">
+        <v>4004</v>
+      </c>
+      <c r="M151" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="N151" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="O151" s="30" t="s">
-        <v>1</v>
+      <c r="O151" s="31" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="152" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A152" s="8">
-        <v>169</v>
+      <c r="A152" s="4">
+        <v>99</v>
       </c>
       <c r="B152" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="C152" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="D152" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E152" s="8" t="s">
+      <c r="C152" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D152" s="4">
+        <v>8</v>
+      </c>
+      <c r="E152" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="F152" s="8" t="s">
+      <c r="F152" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="G152" s="8">
-        <v>401</v>
-      </c>
-      <c r="H152" s="54" t="s">
-        <v>216</v>
+      <c r="G152" s="38">
+        <v>200</v>
+      </c>
+      <c r="H152" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="I152" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="J152" s="92" t="s">
+        <v>228</v>
+      </c>
+      <c r="J152" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K152" s="92" t="s">
-        <v>32</v>
-      </c>
-      <c r="L152" s="8">
-        <v>1014</v>
-      </c>
-      <c r="M152" s="31" t="s">
-        <v>298</v>
+      <c r="K152" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L152" s="4">
+        <v>1010</v>
+      </c>
+      <c r="M152" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="N152" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="O152" s="64" t="s">
-        <v>12</v>
+      <c r="O152" s="30" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:66" ht="18.75" x14ac:dyDescent="0.25">
@@ -35052,8 +35052,8 @@
       <c r="M173" s="31" t="s">
         <v>298</v>
       </c>
-      <c r="N173" s="33" t="s">
-        <v>214</v>
+      <c r="N173" s="64" t="s">
+        <v>12</v>
       </c>
       <c r="O173" s="64" t="s">
         <v>12</v>
@@ -40292,18 +40292,18 @@
     <mergeCell ref="A70:O70"/>
     <mergeCell ref="A153:O153"/>
     <mergeCell ref="A154:O154"/>
-    <mergeCell ref="A145:O145"/>
-    <mergeCell ref="A124:O124"/>
+    <mergeCell ref="A146:O146"/>
+    <mergeCell ref="A125:O125"/>
     <mergeCell ref="A129:O129"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J10:J17 J125:J126 J146:J151 J7:J8 J75:J76 J91:J92 J106:J108 J133:J135 J158:J159 J20:J21 J137:J144 J110:J123 J94:J99 J30 J78:J83 J55:J68 J161:J172 J33:J53" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J10:J17 J126:J127 J147:J152 J7:J8 J75:J76 J91:J92 J106:J108 J133:J135 J158:J159 J20:J21 J137:J145 J110:J124 J94:J99 J30 J78:J83 J55:J68 J161:J172 J33:J53" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Error,Warning"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K146:K148 K10:K17 K151 K125:K126 K7:K8 K75:K76 K91:K92 K106:K108 K133:K135 K158:K159 K20:K21 K78:K83 K137:K144 K110:K123 K94:K99 K55:K68 K161:K172 K30:K53" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K147:K149 K10:K17 K152 K126:K127 K7:K8 K75:K76 K91:K92 K106:K108 K133:K135 K158:K159 K20:K21 K78:K83 K137:K145 K110:K124 K94:K99 K55:K68 K161:K172 K30:K53" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Field,Cross Field,Cross Form"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L10:L15 L20:L21 L110:L116 L94:L99 L126 L55:L59 L165:L167 L161:L163 L7:L8 L75:L76 L91:L92 L106:L108 L133:L135 L158:L159 L17 L43:L52 L78:L83 L137:L139 L141:L144 L33 L30 L148 L151 L35:L41" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L10:L15 L20:L21 L110:L116 L94:L99 L127 L55:L59 L165:L167 L161:L163 L7:L8 L75:L76 L91:L92 L106:L108 L133:L135 L158:L159 L17 L43:L52 L78:L83 L137:L139 L141:L145 L33 L30 L149 L152 L35:L41" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>